<commit_message>
oop changes (more flexible)
</commit_message>
<xml_diff>
--- a/home.xlsx
+++ b/home.xlsx
@@ -16,6 +16,51 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
+    <t>https://www.otodom.pl/oferta/kawalerka-po-remoncie-ID3ULoM.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/kawalerka-przymorze-po-remoncie-z-duzym-balkonem-ID3UL7m.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/tanie-mieszkanie-ciche-i-sloneczne-ID3UKFV.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/cicha-okolica-blisko-obwodnicy-od-zaraz-ID3UIa4.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/sloneczna-kawalerka-z-osobna-kuchnia-ID3UHic.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/mieszkanie-gdansk-jasien-ID3UFQY.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/tbs-sliczne-3-pokoje-po-generalnym-remoncie-ID3UFB2.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/niezalezna-kawalerka-700m-od-plazy-ID3UD8s.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/kawalerka-na-przymorzu-z-balkonem-17m2-209000zl-ID3UAOM.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/2-pokoje-w-dobrej-cenie-ID3UyYk.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/najtansza-ladna-kawalerka-na-zaspie-ID3Uyo0.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/1-pokoj-z-balkonem-i-oddzielna-kuchnia-w-gdansku-ID3UuLu.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/32m2-pruszcz-gd-po-kapitalnym-remoncie-ID3UsBK.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/kawalerka-dostepna-od-zaraz-ID3UrRC.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.otodom.pl/oferta/kawalerka-w-centrum-miasta-w-dobrej-cenie-ID3Uqje.html#115d627921</t>
+  </si>
+  <si>
     <t>https://www.otodom.pl/oferta/2-zadbane-pokoje-na-parterze-pruszcz-ID3UkOA.html#115d627921</t>
   </si>
   <si>
@@ -28,15 +73,6 @@
     <t>https://www.otodom.pl/oferta/kawalerka-na-wyspie-sobieszewskiej-ID3UhDu.html#115d627921</t>
   </si>
   <si>
-    <t>https://www.otodom.pl/oferta/kawalerka-na-zaspie-swietne-lokalizacja-pilotow-ID3UhdK.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/umeblowana-kawalerka-w-bloku-ID3Uhcg.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/kawalerka-blisko-uczelni-inwestycja-ID3UeQo.html#115d627921</t>
-  </si>
-  <si>
     <t>https://www.otodom.pl/oferta/mieszkanie-33-60-m-gdansk-ID3Uc96.html#115d627921</t>
   </si>
   <si>
@@ -50,42 +86,6 @@
   </si>
   <si>
     <t>https://www.otodom.pl/oferta/2-pok-w-kamienicy-blisko-starowki-ID3U4u0.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/600-metrow-do-plazy-brzezno-kawalerka-ID3U3B6.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/sprzedam-1-pokojowe-mieszkanie-w-centrum-wrzeszcza-ID3U0uE.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/na-sprzedaz-trzypokojowe-mieszkanie-w-tczewie-ID3TZqg.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/gotowe-mieszkanie-2-pokojowe-na-jasieniu-ID3TZms.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/sloneczne-2-pok-48m2-w-centrum-ID3TX6g.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/kawalerka-do-zamieszkania-gdansk-wrzeszcz-blok-ID3TR9a.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/sprzedam-2-pok-mieszkanie-na-ul-saperskiej-ID3TQNS.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/przytulna-kawalerka-32-81-m2-ID3TO7m.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/dwa-pokoje-w-idealnej-lokalizacji-ID3TMNS.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/wyremontowana-kawalerka-z-balkonem-17-m2-ID3TMmM.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/kawalerka-na-przymorzu-ID3TLec.html#115d627921</t>
-  </si>
-  <si>
-    <t>https://www.otodom.pl/oferta/2-pokoje-42-42m2-2-pietro-gotowe-do-wprowadzenia-g-ID3TErG.html#115d627921</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
working with several websites(otodom, morizon, adresowo, freedom, metrohouse)
</commit_message>
<xml_diff>
--- a/home.xlsx
+++ b/home.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>https://www.otodom.pl/oferta/kawalerka-po-remoncie-ID3ULoM.html#115d627921</t>
   </si>
@@ -86,6 +86,195 @@
   </si>
   <si>
     <t>https://www.otodom.pl/oferta/2-pok-w-kamienicy-blisko-starowki-ID3U4u0.html#115d627921</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-lodzka-26m2-mzn2032934340</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-brzezno-dworska-25m2-mzn2032929501</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-zabianka-wejhera-jelitkowo-tysiaclecia-wejhera-22m2-mzn2032929581</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-siedlce-kartuska-33m2-mzn2032928910</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-33m2-mzn2032860941</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-pastelowa-36m2-mzn2032779904</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-przymorze-chlopska-30m2-mzn2032779517</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-srodmiescie-zaroslak-28m2-mzn2032778016</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-oliwa-kaszubska-21m2-mzn2032771404</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-jasien-konrada-guderskiego-35m2-mzn2032768993</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-wrzeszcz-partyzantow-23m2-mzn2032767024</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-orunia-sw-wojciech-lipce-trakt-sw-wojciecha-33m2-mzn2032766093</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-niepolomicka-42m2-mzn2032764755</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-siedlce-szara-31m2-mzn2032761832</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-srebrna-55m2-mzn2032760961</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-orunia-sw-wojciech-lipce-trakt-sw-wojciecha-55m2-mzn2032750332</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-siedlce-pobiedzisko-36m2-mzn2032758151</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-siedlce-szara-31m2-mzn2032757238</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-wrzeszcz-zygmunta-augusta-25m2-mzn2032732822</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-jasien-kazimierza-leskiego-31m2-mzn2032731278</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-ujescisko-lostowice-stanislawa-dabka-26m2-mzn2032724768</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-srodmiescie-dlugie-ogrody-26m2-mzn2032721788</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-przymorze-jagiellonska-17m2-mzn2032710489</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-przymorze-gen-bora-komorowskiego-22m2-mzn2032719796</t>
+  </si>
+  <si>
+    <t>https://www.morizon.pl/oferta/sprzedaz-mieszkanie-gdansk-przymorze-jagiellonska-17m2-mzn2032719716</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/n7g3n3</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/z8u8f8</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/q4m4f8</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/w3x1j8</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/r8j4s1</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/s1u1r9</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/y0q5x6</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/a3v8s2</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/g5r9x0</t>
+  </si>
+  <si>
+    <t>https://adresowo.pl/o/v7k1w3</t>
+  </si>
+  <si>
+    <t>https://www.freedom-nieruchomosci.pl/oferta/14371-3685-OMS</t>
+  </si>
+  <si>
+    <t>https://www.freedom-nieruchomosci.pl/oferta/13474-3685-OMS</t>
+  </si>
+  <si>
+    <t>https://www.freedom-nieruchomosci.pl/oferta/12209-3685-OMS</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/XEFA995/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/DOTI672/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/GIRE819/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/MIME686/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/JYTY517/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/MIKA808/nieruchomosc-na-sprzedaz-mieszkanie---</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/NYPI996/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-lostowice-niepolomicka</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/HIFU496/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/DUKA399/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-jasien-jabloniowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/BETI294/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-jasien-jabloniowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/RATY916/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-przymorze-jagiellonska</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/LOJU145/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/KAMU925/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/DABO949/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/GIXE939/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/XAXE929/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/NYCY486/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/JIHE919/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/MYSE782/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/HUBA481/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/HOKA492/nieruchomosc-na-sprzedaz-mieszkanie---pastelowa</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/PUKI611/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-kielpinek-przytulna</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/BOCE261/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-kielpinek-przytulna</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/KITU667/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-kielpinek-przytulna</t>
+  </si>
+  <si>
+    <t>https://metrohouse.pl/nieruchomosc/HYPO634/nieruchomosc-na-sprzedaz-mieszkanie-gdansk-kielpinek-przytulna</t>
   </si>
 </sst>
 </file>
@@ -430,158 +619,412 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
+      <c r="B22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="115d627921"/>
-    <hyperlink ref="A2" r:id="rId2" location="115d627921"/>
-    <hyperlink ref="A3" r:id="rId3" location="115d627921"/>
-    <hyperlink ref="A4" r:id="rId4" location="115d627921"/>
-    <hyperlink ref="A5" r:id="rId5" location="115d627921"/>
-    <hyperlink ref="A6" r:id="rId6" location="115d627921"/>
-    <hyperlink ref="A7" r:id="rId7" location="115d627921"/>
-    <hyperlink ref="A8" r:id="rId8" location="115d627921"/>
-    <hyperlink ref="A9" r:id="rId9" location="115d627921"/>
-    <hyperlink ref="A10" r:id="rId10" location="115d627921"/>
-    <hyperlink ref="A11" r:id="rId11" location="115d627921"/>
-    <hyperlink ref="A12" r:id="rId12" location="115d627921"/>
-    <hyperlink ref="A13" r:id="rId13" location="115d627921"/>
-    <hyperlink ref="A14" r:id="rId14" location="115d627921"/>
-    <hyperlink ref="A15" r:id="rId15" location="115d627921"/>
-    <hyperlink ref="A16" r:id="rId16" location="115d627921"/>
-    <hyperlink ref="A17" r:id="rId17" location="115d627921"/>
-    <hyperlink ref="A18" r:id="rId18" location="115d627921"/>
-    <hyperlink ref="A19" r:id="rId19" location="115d627921"/>
-    <hyperlink ref="A20" r:id="rId20" location="115d627921"/>
-    <hyperlink ref="A21" r:id="rId21" location="115d627921"/>
-    <hyperlink ref="A22" r:id="rId22" location="115d627921"/>
-    <hyperlink ref="A23" r:id="rId23" location="115d627921"/>
-    <hyperlink ref="A24" r:id="rId24" location="115d627921"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="C1" r:id="rId3"/>
+    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="E1" r:id="rId5"/>
+    <hyperlink ref="A2" r:id="rId6" location="115d627921"/>
+    <hyperlink ref="B2" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
+    <hyperlink ref="D2" r:id="rId9"/>
+    <hyperlink ref="E2" r:id="rId10"/>
+    <hyperlink ref="A3" r:id="rId11" location="115d627921"/>
+    <hyperlink ref="B3" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="D3" r:id="rId14"/>
+    <hyperlink ref="E3" r:id="rId15"/>
+    <hyperlink ref="A4" r:id="rId16" location="115d627921"/>
+    <hyperlink ref="B4" r:id="rId17"/>
+    <hyperlink ref="C4" r:id="rId18"/>
+    <hyperlink ref="E4" r:id="rId19"/>
+    <hyperlink ref="A5" r:id="rId20" location="115d627921"/>
+    <hyperlink ref="B5" r:id="rId21"/>
+    <hyperlink ref="C5" r:id="rId22"/>
+    <hyperlink ref="E5" r:id="rId23"/>
+    <hyperlink ref="A6" r:id="rId24" location="115d627921"/>
+    <hyperlink ref="B6" r:id="rId25"/>
+    <hyperlink ref="C6" r:id="rId26"/>
+    <hyperlink ref="E6" r:id="rId27"/>
+    <hyperlink ref="A7" r:id="rId28" location="115d627921"/>
+    <hyperlink ref="B7" r:id="rId29"/>
+    <hyperlink ref="C7" r:id="rId30"/>
+    <hyperlink ref="E7" r:id="rId31"/>
+    <hyperlink ref="A8" r:id="rId32" location="115d627921"/>
+    <hyperlink ref="B8" r:id="rId33"/>
+    <hyperlink ref="C8" r:id="rId34"/>
+    <hyperlink ref="E8" r:id="rId35"/>
+    <hyperlink ref="A9" r:id="rId36" location="115d627921"/>
+    <hyperlink ref="B9" r:id="rId37"/>
+    <hyperlink ref="C9" r:id="rId38"/>
+    <hyperlink ref="E9" r:id="rId39"/>
+    <hyperlink ref="A10" r:id="rId40" location="115d627921"/>
+    <hyperlink ref="B10" r:id="rId41"/>
+    <hyperlink ref="C10" r:id="rId42"/>
+    <hyperlink ref="E10" r:id="rId43"/>
+    <hyperlink ref="A11" r:id="rId44" location="115d627921"/>
+    <hyperlink ref="B11" r:id="rId45"/>
+    <hyperlink ref="E11" r:id="rId46"/>
+    <hyperlink ref="A12" r:id="rId47" location="115d627921"/>
+    <hyperlink ref="B12" r:id="rId48"/>
+    <hyperlink ref="E12" r:id="rId49"/>
+    <hyperlink ref="A13" r:id="rId50" location="115d627921"/>
+    <hyperlink ref="B13" r:id="rId51"/>
+    <hyperlink ref="E13" r:id="rId52"/>
+    <hyperlink ref="A14" r:id="rId53" location="115d627921"/>
+    <hyperlink ref="B14" r:id="rId54"/>
+    <hyperlink ref="E14" r:id="rId55"/>
+    <hyperlink ref="A15" r:id="rId56" location="115d627921"/>
+    <hyperlink ref="B15" r:id="rId57"/>
+    <hyperlink ref="E15" r:id="rId58"/>
+    <hyperlink ref="A16" r:id="rId59" location="115d627921"/>
+    <hyperlink ref="B16" r:id="rId60"/>
+    <hyperlink ref="E16" r:id="rId61"/>
+    <hyperlink ref="A17" r:id="rId62" location="115d627921"/>
+    <hyperlink ref="B17" r:id="rId63"/>
+    <hyperlink ref="E17" r:id="rId64"/>
+    <hyperlink ref="A18" r:id="rId65" location="115d627921"/>
+    <hyperlink ref="B18" r:id="rId66"/>
+    <hyperlink ref="E18" r:id="rId67"/>
+    <hyperlink ref="A19" r:id="rId68" location="115d627921"/>
+    <hyperlink ref="B19" r:id="rId69"/>
+    <hyperlink ref="E19" r:id="rId70"/>
+    <hyperlink ref="A20" r:id="rId71" location="115d627921"/>
+    <hyperlink ref="B20" r:id="rId72"/>
+    <hyperlink ref="E20" r:id="rId73"/>
+    <hyperlink ref="A21" r:id="rId74" location="115d627921"/>
+    <hyperlink ref="B21" r:id="rId75"/>
+    <hyperlink ref="E21" r:id="rId76"/>
+    <hyperlink ref="A22" r:id="rId77" location="115d627921"/>
+    <hyperlink ref="B22" r:id="rId78"/>
+    <hyperlink ref="E22" r:id="rId79"/>
+    <hyperlink ref="A23" r:id="rId80" location="115d627921"/>
+    <hyperlink ref="B23" r:id="rId81"/>
+    <hyperlink ref="E23" r:id="rId82"/>
+    <hyperlink ref="A24" r:id="rId83" location="115d627921"/>
+    <hyperlink ref="B24" r:id="rId84"/>
+    <hyperlink ref="E24" r:id="rId85"/>
+    <hyperlink ref="B25" r:id="rId86"/>
+    <hyperlink ref="E25" r:id="rId87"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>